<commit_message>
index match vs Vlookup
</commit_message>
<xml_diff>
--- a/4. INDEX_MATCH  vs VLOOKUP.xlsx
+++ b/4. INDEX_MATCH  vs VLOOKUP.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\GitHub_Clone_Repo\Rahul_Repo\Me_Mastering_Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pande\Desktop\GitHub_Clone\Me_Mastering_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE848190-406C-4EB7-97E1-955C5D4536F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E76E746-38A2-45DF-9200-1C304065543E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{83BDEA4C-27AA-45C6-8A81-0092FB6AC14B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{83BDEA4C-27AA-45C6-8A81-0092FB6AC14B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Theory" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -413,6 +414,197 @@
             <a:t> stock price of TCS on 2-Mar-2024 = </a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD53BAE3-72D8-C3A5-0656-F19229CB2CA3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="701040" y="160020"/>
+          <a:ext cx="12321540" cy="4709160"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t># Difference Between VLOOKUP and INDEX-MATCH in Excel</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-IN" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>## 🔹 VLOOKUP (Vertical Lookup)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>- Looks up a value in the first column of a table and returns a value from another column.  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>- Can **only look to the right** of the lookup column.  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>- Requires a **column index number** to specify which column to return data from.  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>- If columns are inserted or deleted, the formula may break.  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>- Works only in a **vertical direction**.  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-IN" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>---</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-IN" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>## 🔹 INDEX + MATCH Combination</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>- A flexible alternative that uses MATCH to find a position and INDEX to return a value.  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>- Can **look left or right**, unlike VLOOKUP.  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>- More **dynamic and flexible**, since MATCH finds the position automatically.  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>- Works both **vertically and horizontally**.  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>- Generally **faster and more reliable** than VLOOKUP on large datasets.  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-IN" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>---</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-IN" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>## 🔹 When to Use What?</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>- Use **VLOOKUP** → for **quick, simple lookups** when data is stable.  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>- Use **INDEX + MATCH** → for **flexibility, large datasets, and when columns may change**.  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-IN" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -752,16 +944,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B4729B-F267-40ED-9E43-74BD766CCB62}">
   <dimension ref="C10:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C10" s="1" t="s">
         <v>0</v>
       </c>
@@ -772,7 +964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C11" s="2">
         <v>45352</v>
       </c>
@@ -783,7 +975,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C12" s="2">
         <v>45353</v>
       </c>
@@ -794,7 +986,7 @@
         <v>1450</v>
       </c>
     </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C13" s="2">
         <v>45352</v>
       </c>
@@ -805,7 +997,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C14" s="2">
         <v>45353</v>
       </c>
@@ -816,7 +1008,7 @@
         <v>3520</v>
       </c>
     </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C15" s="2">
         <v>45354</v>
       </c>
@@ -827,7 +1019,7 @@
         <v>1460</v>
       </c>
     </row>
-    <row r="17" spans="15:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="15:15" x14ac:dyDescent="0.3">
       <c r="O17" cm="1">
         <f t="array" ref="O17">INDEX(Table1[Stock Prices], MATCH(1,(Table1[Compnay]="TCS")*(Table1[Date]=DATE(2024,3,2)),0))</f>
         <v>3520</v>
@@ -840,4 +1032,19 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F9512CF-2CBD-4B51-98F2-655F17F6EE6C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>